<commit_message>
Found and fixed SearchCommand and StreamingCommand bugs
Also added a smoke test and improved the countmatches example some.
</commit_message>
<xml_diff>
--- a/Commands.conf.spec.xlsx
+++ b/Commands.conf.spec.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25516"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="25808"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/david-noble/Workspace/splunk-mine/splunk-sdk-python/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15820" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +17,7 @@
   <definedNames>
     <definedName name="commands.conf" localSheetId="0">Sheet1!$A$3:$A$124</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -616,6 +621,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -965,10 +975,10 @@
   <dimension ref="A1:H123"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="113.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -980,7 +990,7 @@
     <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="13" t="s">
@@ -996,7 +1006,7 @@
       </c>
       <c r="H1" s="13"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>80</v>
       </c>
@@ -1022,7 +1032,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1038,7 +1048,7 @@
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
         <v>1</v>
       </c>
@@ -1050,7 +1060,7 @@
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
         <v>2</v>
       </c>
@@ -1062,7 +1072,7 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -1078,7 +1088,7 @@
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>4</v>
       </c>
@@ -1090,17 +1100,17 @@
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1124,7 +1134,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="10" t="s">
         <v>8</v>
       </c>
@@ -1136,7 +1146,7 @@
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
         <v>9</v>
       </c>
@@ -1148,7 +1158,7 @@
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>10</v>
       </c>
@@ -1174,17 +1184,17 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
@@ -1211,7 +1221,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="10" t="s">
         <v>17</v>
       </c>
@@ -1223,22 +1233,22 @@
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>21</v>
       </c>
@@ -1267,7 +1277,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>109</v>
       </c>
@@ -1279,20 +1289,20 @@
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>22</v>
       </c>
@@ -1321,17 +1331,17 @@
         <v>85</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>23</v>
       </c>
@@ -1360,7 +1370,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="10" t="s">
         <v>24</v>
       </c>
@@ -1372,27 +1382,27 @@
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>48</v>
       </c>
@@ -1421,7 +1431,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="10" t="s">
         <v>49</v>
       </c>
@@ -1433,22 +1443,22 @@
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="10" t="s">
         <v>53</v>
       </c>
@@ -1460,7 +1470,7 @@
       <c r="G46" s="10"/>
       <c r="H46" s="10"/>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>54</v>
       </c>
@@ -1476,7 +1486,7 @@
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="10" t="s">
         <v>55</v>
       </c>
@@ -1488,12 +1498,12 @@
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>57</v>
       </c>
@@ -1509,12 +1519,12 @@
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="12" t="s">
         <v>105</v>
       </c>
@@ -1526,7 +1536,7 @@
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="12" t="s">
         <v>100</v>
       </c>
@@ -1538,7 +1548,7 @@
       <c r="G55" s="10"/>
       <c r="H55" s="10"/>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>58</v>
       </c>
@@ -1567,12 +1577,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="12" t="s">
         <v>102</v>
       </c>
@@ -1584,7 +1594,7 @@
       <c r="G59" s="10"/>
       <c r="H59" s="10"/>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="12" t="s">
         <v>103</v>
       </c>
@@ -1596,15 +1606,15 @@
       <c r="G60" s="10"/>
       <c r="H60" s="10"/>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="11"/>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>59</v>
       </c>
@@ -1633,7 +1643,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="10" t="s">
         <v>60</v>
       </c>
@@ -1645,12 +1655,12 @@
       <c r="G64" s="10"/>
       <c r="H64" s="10"/>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>62</v>
       </c>
@@ -1679,17 +1689,17 @@
         <v>85</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>65</v>
       </c>
@@ -1718,7 +1728,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" s="10" t="s">
         <v>66</v>
       </c>
@@ -1730,17 +1740,17 @@
       <c r="G72" s="10"/>
       <c r="H72" s="10"/>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>73</v>
       </c>
@@ -1769,22 +1779,22 @@
         <v>85</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" s="10" t="s">
         <v>77</v>
       </c>
@@ -1796,7 +1806,7 @@
       <c r="G80" s="10"/>
       <c r="H80" s="10"/>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" s="10" t="s">
         <v>78</v>
       </c>
@@ -1808,12 +1818,12 @@
       <c r="G81" s="10"/>
       <c r="H81" s="10"/>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>13</v>
       </c>
@@ -1842,17 +1852,17 @@
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>29</v>
       </c>
@@ -1881,22 +1891,22 @@
         <v>85</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>31</v>
       </c>
@@ -1925,7 +1935,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" s="10" t="s">
         <v>32</v>
       </c>
@@ -1937,7 +1947,7 @@
       <c r="G94" s="10"/>
       <c r="H94" s="10"/>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" s="10" t="s">
         <v>33</v>
       </c>
@@ -1949,7 +1959,7 @@
       <c r="G95" s="10"/>
       <c r="H95" s="10"/>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" s="10" t="s">
         <v>15</v>
       </c>
@@ -1961,7 +1971,7 @@
       <c r="G96" s="10"/>
       <c r="H96" s="10"/>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>34</v>
       </c>
@@ -1980,7 +1990,7 @@
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="10" t="s">
         <v>35</v>
       </c>
@@ -1992,12 +2002,12 @@
       <c r="G99" s="10"/>
       <c r="H99" s="10"/>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>36</v>
       </c>
@@ -2016,17 +2026,17 @@
         <v>85</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>38</v>
       </c>
@@ -2043,7 +2053,7 @@
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="10" t="s">
         <v>39</v>
       </c>
@@ -2055,12 +2065,12 @@
       <c r="G107" s="10"/>
       <c r="H107" s="10"/>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="10" t="s">
         <v>41</v>
       </c>
@@ -2072,7 +2082,7 @@
       <c r="G109" s="10"/>
       <c r="H109" s="10"/>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>42</v>
       </c>
@@ -2090,12 +2100,12 @@
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>44</v>
       </c>
@@ -2121,7 +2131,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="10" t="s">
         <v>45</v>
       </c>
@@ -2133,17 +2143,17 @@
       <c r="G115" s="10"/>
       <c r="H115" s="10"/>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A119" s="3" t="s">
         <v>69</v>
       </c>
@@ -2172,22 +2182,22 @@
         <v>85</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A123" s="10" t="s">
         <v>68</v>
       </c>
@@ -2210,10 +2220,5 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
We now correctly record inputs and outputs when record=true is specified as a search command options
Next up: ensure we can utilize such recordings in tests.
</commit_message>
<xml_diff>
--- a/Commands.conf.spec.xlsx
+++ b/Commands.conf.spec.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="25808"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="25924"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="commands.conf" localSheetId="0">Sheet1!$A$3:$A$124</definedName>
+    <definedName name="commands.conf" localSheetId="0">Sheet1!$B$3:$B$124</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="113">
   <si>
     <t>type = &lt;string&gt;</t>
   </si>
@@ -382,6 +382,9 @@
   </si>
   <si>
     <t>* Defaults to true</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -634,9 +637,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:H124" totalsRowShown="0">
-  <autoFilter ref="A2:H124"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:I124" totalsRowShown="0">
+  <autoFilter ref="A2:I124"/>
+  <tableColumns count="9">
+    <tableColumn id="9" name="N"/>
     <tableColumn id="1" name="Configuration setting"/>
     <tableColumn id="8" name="Settable from"/>
     <tableColumn id="2" name="Default [GC]"/>
@@ -972,25 +976,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H123"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="113.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
+    <col min="7" max="7" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="13" t="s">
@@ -1006,1208 +1011,1322 @@
       </c>
       <c r="H1" s="13"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" t="s">
         <v>80</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>94</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>86</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>87</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>88</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>89</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>90</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="7" t="s">
+      <c r="D3" s="6"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
+      <c r="I3" s="6"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="10"/>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="I4" s="10"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="10"/>
       <c r="C5" s="10"/>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="I5" s="10"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="10"/>
+      <c r="B8" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="10"/>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="I8" s="10"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>3</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="C12" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C12" s="2" t="str">
+      <c r="D12" s="2" t="str">
         <f>"false"</f>
         <v>false</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2" t="str">
+      <c r="E12" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2" t="str">
         <f>"false"</f>
         <v>false</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
+      <c r="I12" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="I13" s="10"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="10"/>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="3" t="s">
+      <c r="I14" s="10"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>4</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C16" s="4">
+      <c r="D16" s="4">
         <v>0</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E16" s="4">
+      <c r="E16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="4">
         <v>0</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G16" s="4">
+      <c r="G16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" s="4">
         <v>0</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="I16" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="3" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>5</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="4">
+      <c r="D20" s="4">
         <v>0</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" s="4">
+      <c r="E20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F20" s="4">
         <v>0</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G20" s="4">
+      <c r="G20" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H20" s="4">
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="H20" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" s="10" t="s">
+      <c r="I20" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="10"/>
+      <c r="B21" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="10"/>
       <c r="C21" s="10"/>
       <c r="D21" s="10"/>
       <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="I21" s="10"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>6</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C26" s="2" t="str">
+      <c r="D26" s="2" t="str">
         <f>"false"</f>
         <v>false</v>
       </c>
-      <c r="D26" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E26" s="2" t="str">
+      <c r="E26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" s="2" t="str">
         <f>"false"</f>
         <v>false</v>
       </c>
-      <c r="F26" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G26" s="2" t="str">
+      <c r="G26" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" s="2" t="str">
         <f>"false"</f>
         <v>false</v>
       </c>
-      <c r="H26" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="12" t="s">
+      <c r="I26" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="B27" s="10"/>
       <c r="C27" s="10"/>
       <c r="D27" s="10"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="11" t="s">
+      <c r="I27" s="10"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="11"/>
+      <c r="B28" s="11" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="11"/>
+      <c r="B29" s="11" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="11"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
+      <c r="B30" s="11"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>7</v>
+      </c>
+      <c r="B31" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="C31" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C31" s="2" t="str">
+      <c r="D31" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E31" s="2" t="str">
+      <c r="E31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F31" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="F31" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G31" s="2" t="str">
+      <c r="G31" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H31" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="H31" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="11" t="s">
+      <c r="I31" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="11" t="s">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
+      <c r="B33" s="11" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="3" t="s">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>8</v>
+      </c>
+      <c r="B35" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C35" s="2" t="str">
+      <c r="D35" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E35" s="2" t="str">
+      <c r="F35" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G35" s="2" t="str">
+      <c r="H35" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="H35" s="2" t="s">
+      <c r="I35" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="10" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="10"/>
       <c r="C36" s="10"/>
       <c r="D36" s="10"/>
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
       <c r="H36" s="10"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="I36" s="10"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>9</v>
+      </c>
+      <c r="B41" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="C41" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C41" s="2" t="str">
+      <c r="D41" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E41" s="2" t="str">
+      <c r="F41" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="G41" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G41" s="2" t="str">
+      <c r="H41" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="H41" s="2" t="s">
+      <c r="I41" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="10" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+      <c r="B42" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="B42" s="10"/>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
       <c r="F42" s="10"/>
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
+      <c r="I42" s="10"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="10" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+      <c r="B46" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="B46" s="10"/>
       <c r="C46" s="10"/>
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
       <c r="G46" s="10"/>
       <c r="H46" s="10"/>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
+      <c r="I46" s="10"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>10</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="C48" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C48" s="6"/>
       <c r="D48" s="6"/>
-      <c r="E48" s="9" t="s">
+      <c r="E48" s="6"/>
+      <c r="F48" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="F48" s="6"/>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="10" t="s">
+      <c r="I48" s="6"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
+      <c r="B49" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="B49" s="10"/>
       <c r="C49" s="10"/>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
       <c r="G49" s="10"/>
       <c r="H49" s="10"/>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" t="s">
+      <c r="I49" s="10"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B50" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="3" t="s">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>11</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="C52" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C52" s="6"/>
       <c r="D52" s="6"/>
-      <c r="E52" s="9" t="s">
+      <c r="E52" s="6"/>
+      <c r="F52" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="F52" s="6"/>
       <c r="G52" s="6"/>
       <c r="H52" s="6"/>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="11" t="s">
+      <c r="I52" s="6"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="11"/>
+      <c r="B53" s="11" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="12" t="s">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="12"/>
+      <c r="B54" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="B54" s="10"/>
       <c r="C54" s="10"/>
       <c r="D54" s="10"/>
       <c r="E54" s="10"/>
       <c r="F54" s="10"/>
       <c r="G54" s="10"/>
       <c r="H54" s="10"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="12" t="s">
+      <c r="I54" s="10"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="12"/>
+      <c r="B55" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="B55" s="10"/>
       <c r="C55" s="10"/>
       <c r="D55" s="10"/>
       <c r="E55" s="10"/>
       <c r="F55" s="10"/>
       <c r="G55" s="10"/>
       <c r="H55" s="10"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" s="3" t="s">
+      <c r="I55" s="10"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>12</v>
+      </c>
+      <c r="B57" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B57" s="3" t="s">
+      <c r="C57" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C57" s="2" t="str">
+      <c r="D57" s="2" t="str">
         <f>"false"</f>
         <v>false</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E57" s="2" t="str">
+      <c r="E57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F57" s="2" t="str">
         <f>"false"</f>
         <v>false</v>
       </c>
-      <c r="F57" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G57" s="2" t="str">
+      <c r="G57" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H57" s="2" t="str">
         <f>"false"</f>
         <v>false</v>
       </c>
-      <c r="H57" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" s="11" t="s">
+      <c r="I57" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="11"/>
+      <c r="B58" s="11" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A59" s="12" t="s">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="12"/>
+      <c r="B59" s="12" t="s">
         <v>102</v>
       </c>
-      <c r="B59" s="10"/>
       <c r="C59" s="10"/>
       <c r="D59" s="10"/>
       <c r="E59" s="10"/>
       <c r="F59" s="10"/>
       <c r="G59" s="10"/>
       <c r="H59" s="10"/>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A60" s="12" t="s">
+      <c r="I59" s="10"/>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A60" s="12"/>
+      <c r="B60" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B60" s="10"/>
       <c r="C60" s="10"/>
       <c r="D60" s="10"/>
       <c r="E60" s="10"/>
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
       <c r="H60" s="10"/>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A61" s="11" t="s">
+      <c r="I60" s="10"/>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="11"/>
+      <c r="B61" s="11" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="11"/>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A63" s="3" t="s">
+      <c r="B62" s="11"/>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>13</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B63" s="3" t="s">
+      <c r="C63" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C63" s="2" t="str">
+      <c r="D63" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E63" s="2" t="str">
+      <c r="E63" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F63" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="F63" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G63" s="2" t="str">
+      <c r="G63" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H63" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="H63" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" s="10" t="s">
+      <c r="I63" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A64" s="10"/>
+      <c r="B64" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="B64" s="10"/>
       <c r="C64" s="10"/>
       <c r="D64" s="10"/>
       <c r="E64" s="10"/>
       <c r="F64" s="10"/>
       <c r="G64" s="10"/>
       <c r="H64" s="10"/>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
+      <c r="I64" s="10"/>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A67" s="3" t="s">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>14</v>
+      </c>
+      <c r="B67" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B67" s="3" t="s">
+      <c r="C67" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C67" s="2" t="str">
+      <c r="D67" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="D67" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E67" s="2" t="str">
+      <c r="E67" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F67" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="F67" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G67" s="2" t="str">
+      <c r="G67" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H67" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="H67" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A68" t="s">
+      <c r="I67" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A69" t="s">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A71" s="3" t="s">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
+        <v>15</v>
+      </c>
+      <c r="B71" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="C71" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C71" s="2" t="str">
+      <c r="D71" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="E71" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E71" s="2" t="str">
+      <c r="F71" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="G71" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G71" s="2" t="str">
+      <c r="H71" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="H71" s="2" t="s">
+      <c r="I71" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A72" s="10" t="s">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A72" s="10"/>
+      <c r="B72" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="B72" s="10"/>
       <c r="C72" s="10"/>
       <c r="D72" s="10"/>
       <c r="E72" s="10"/>
       <c r="F72" s="10"/>
       <c r="G72" s="10"/>
       <c r="H72" s="10"/>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A73" t="s">
+      <c r="I72" s="10"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" s="3" t="s">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
+        <v>16</v>
+      </c>
+      <c r="B76" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B76" s="3" t="s">
+      <c r="C76" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C76" s="2" t="str">
+      <c r="D76" s="2" t="str">
         <f>"log"</f>
         <v>log</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E76" s="2" t="str">
+      <c r="E76" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F76" s="2" t="str">
         <f>"log"</f>
         <v>log</v>
       </c>
-      <c r="F76" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G76" s="2" t="str">
+      <c r="G76" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H76" s="2" t="str">
         <f>"log"</f>
         <v>log</v>
       </c>
-      <c r="H76" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
+      <c r="I76" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A79" t="s">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A80" s="10" t="s">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A80" s="10"/>
+      <c r="B80" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="B80" s="10"/>
       <c r="C80" s="10"/>
       <c r="D80" s="10"/>
       <c r="E80" s="10"/>
       <c r="F80" s="10"/>
       <c r="G80" s="10"/>
       <c r="H80" s="10"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A81" s="10" t="s">
+      <c r="I80" s="10"/>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A81" s="10"/>
+      <c r="B81" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B81" s="10"/>
       <c r="C81" s="10"/>
       <c r="D81" s="10"/>
       <c r="E81" s="10"/>
       <c r="F81" s="10"/>
       <c r="G81" s="10"/>
       <c r="H81" s="10"/>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
+      <c r="I81" s="10"/>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A84" s="3" t="s">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A84" s="3">
+        <v>17</v>
+      </c>
+      <c r="B84" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B84" s="3" t="s">
+      <c r="C84" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C84" s="2" t="str">
+      <c r="D84" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="D84" s="2" t="s">
+      <c r="E84" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E84" s="2" t="str">
+      <c r="F84" s="2" t="str">
         <f>"false"</f>
         <v>false</v>
       </c>
-      <c r="F84" s="2" t="s">
+      <c r="G84" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G84" s="2" t="str">
+      <c r="H84" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="H84" s="2" t="s">
+      <c r="I84" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A85" t="s">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A86" t="s">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A88" s="3" t="s">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A88" s="3">
+        <v>18</v>
+      </c>
+      <c r="B88" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B88" s="3" t="s">
+      <c r="C88" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C88" s="2" t="str">
+      <c r="D88" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="D88" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E88" s="2" t="str">
+      <c r="E88" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F88" s="2" t="str">
         <f>"false"</f>
         <v>false</v>
       </c>
-      <c r="F88" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G88" s="2" t="str">
+      <c r="G88" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H88" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="H88" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A89" t="s">
+      <c r="I88" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A90" t="s">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A91" t="s">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A93" s="3" t="s">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A93" s="3">
+        <v>19</v>
+      </c>
+      <c r="B93" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B93" s="3" t="s">
+      <c r="C93" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C93" s="2" t="str">
+      <c r="D93" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="D93" s="2" t="s">
+      <c r="E93" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E93" s="2" t="str">
+      <c r="F93" s="2" t="str">
         <f>"false"</f>
         <v>false</v>
       </c>
-      <c r="F93" s="2" t="s">
+      <c r="G93" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G93" s="2" t="str">
+      <c r="H93" s="2" t="str">
         <f>"false"</f>
         <v>false</v>
       </c>
-      <c r="H93" s="2" t="s">
+      <c r="I93" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A94" s="10" t="s">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A94" s="10"/>
+      <c r="B94" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B94" s="10"/>
       <c r="C94" s="10"/>
       <c r="D94" s="10"/>
       <c r="E94" s="10"/>
       <c r="F94" s="10"/>
       <c r="G94" s="10"/>
       <c r="H94" s="10"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A95" s="10" t="s">
+      <c r="I94" s="10"/>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A95" s="10"/>
+      <c r="B95" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B95" s="10"/>
       <c r="C95" s="10"/>
       <c r="D95" s="10"/>
       <c r="E95" s="10"/>
       <c r="F95" s="10"/>
       <c r="G95" s="10"/>
       <c r="H95" s="10"/>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A96" s="10" t="s">
+      <c r="I95" s="10"/>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A96" s="10"/>
+      <c r="B96" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B96" s="10"/>
       <c r="C96" s="10"/>
       <c r="D96" s="10"/>
       <c r="E96" s="10"/>
       <c r="F96" s="10"/>
       <c r="G96" s="10"/>
       <c r="H96" s="10"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A98" s="3" t="s">
+      <c r="I96" s="10"/>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A98" s="3">
+        <v>20</v>
+      </c>
+      <c r="B98" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B98" s="3" t="s">
+      <c r="C98" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C98" s="2" t="str">
+      <c r="D98" s="2" t="str">
         <f>"false"</f>
         <v>false</v>
       </c>
-      <c r="D98" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E98" s="2"/>
+      <c r="E98" s="2" t="s">
+        <v>85</v>
+      </c>
       <c r="F98" s="2"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A99" s="10" t="s">
+      <c r="I98" s="2"/>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A99" s="10"/>
+      <c r="B99" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B99" s="10"/>
       <c r="C99" s="10"/>
       <c r="D99" s="10"/>
       <c r="E99" s="10"/>
       <c r="F99" s="10"/>
       <c r="G99" s="10"/>
       <c r="H99" s="10"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A100" t="s">
+      <c r="I99" s="10"/>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B100" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A102" s="3" t="s">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A102" s="3">
+        <v>21</v>
+      </c>
+      <c r="B102" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B102" s="3" t="s">
+      <c r="C102" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C102" s="2"/>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
       <c r="F102" s="2"/>
-      <c r="G102" s="2" t="str">
+      <c r="G102" s="2"/>
+      <c r="H102" s="2" t="str">
         <f>"false"</f>
         <v>false</v>
       </c>
-      <c r="H102" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A103" t="s">
+      <c r="I102" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A104" t="s">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B104" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A106" s="3" t="s">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A106" s="3">
+        <v>22</v>
+      </c>
+      <c r="B106" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B106" s="3" t="s">
+      <c r="C106" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C106" s="2"/>
       <c r="D106" s="2"/>
-      <c r="E106" s="2" t="str">
+      <c r="E106" s="2"/>
+      <c r="F106" s="2" t="str">
         <f>"false"</f>
         <v>false</v>
       </c>
-      <c r="F106" s="2"/>
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A107" s="10" t="s">
+      <c r="I106" s="2"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A107" s="10"/>
+      <c r="B107" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B107" s="10"/>
       <c r="C107" s="10"/>
       <c r="D107" s="10"/>
       <c r="E107" s="10"/>
       <c r="F107" s="10"/>
       <c r="G107" s="10"/>
       <c r="H107" s="10"/>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
+      <c r="I107" s="10"/>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A109" s="10" t="s">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A109" s="10"/>
+      <c r="B109" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B109" s="10"/>
       <c r="C109" s="10"/>
       <c r="D109" s="10"/>
       <c r="E109" s="10"/>
       <c r="F109" s="10"/>
       <c r="G109" s="10"/>
       <c r="H109" s="10"/>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A111" s="3" t="s">
+      <c r="I109" s="10"/>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A111" s="3">
+        <v>23</v>
+      </c>
+      <c r="B111" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B111" s="3" t="s">
+      <c r="C111" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C111" s="2"/>
       <c r="D111" s="2"/>
-      <c r="E111" s="5" t="s">
+      <c r="E111" s="2"/>
+      <c r="F111" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F111" s="2" t="s">
+      <c r="G111" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G111" s="2"/>
       <c r="H111" s="2"/>
-    </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A112" t="s">
+      <c r="I111" s="2"/>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A114" s="3" t="s">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A114" s="3">
+        <v>24</v>
+      </c>
+      <c r="B114" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B114" s="3" t="s">
+      <c r="C114" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C114" s="5" t="s">
+      <c r="D114" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="D114" s="2" t="s">
+      <c r="E114" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E114" s="5" t="s">
+      <c r="F114" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="F114" s="2" t="s">
+      <c r="G114" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G114" s="5" t="s">
+      <c r="H114" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="H114" s="2" t="s">
+      <c r="I114" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A115" s="10" t="s">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A115" s="10"/>
+      <c r="B115" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B115" s="10"/>
       <c r="C115" s="10"/>
       <c r="D115" s="10"/>
       <c r="E115" s="10"/>
       <c r="F115" s="10"/>
       <c r="G115" s="10"/>
       <c r="H115" s="10"/>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
+      <c r="I115" s="10"/>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A117" t="s">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A119" s="3" t="s">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A119" s="3">
+        <v>25</v>
+      </c>
+      <c r="B119" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="C119" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C119" s="2" t="str">
+      <c r="D119" s="2" t="str">
         <f>"false"</f>
         <v>false</v>
       </c>
-      <c r="D119" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E119" s="2" t="str">
+      <c r="E119" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="F119" s="2" t="str">
         <f>"true"</f>
         <v>true</v>
       </c>
-      <c r="F119" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="G119" s="2" t="str">
+      <c r="G119" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H119" s="2" t="str">
         <f>"false"</f>
         <v>false</v>
       </c>
-      <c r="H119" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A120" t="s">
+      <c r="I119" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A121" t="s">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A122" t="s">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A123" s="10" t="s">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A123" s="10"/>
+      <c r="B123" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B123" s="10"/>
       <c r="C123" s="10"/>
       <c r="D123" s="10"/>
       <c r="E123" s="10"/>
       <c r="F123" s="10"/>
       <c r="G123" s="10"/>
       <c r="H123" s="10"/>
+      <c r="I123" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
Minor refactoring + spreadsheet update + todo removal
</commit_message>
<xml_diff>
--- a/Commands.conf.spec.xlsx
+++ b/Commands.conf.spec.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28260" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="commands.conf" localSheetId="0">Sheet1!$B$3:$B$124</definedName>
@@ -24,6 +25,40 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="G8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Based on presence of a ReportingCommand.map method annotated with the Configuration decorator. If there is no map method, streaming_preop is None and requires_preop is ignored.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Ignored unless type='streaming'. Only streaming commands can be distributed.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
@@ -46,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="142">
   <si>
     <t>type = &lt;string&gt;</t>
   </si>
@@ -385,13 +420,100 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Settiing</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>unicode</t>
+  </si>
+  <si>
+    <t>SCP v1</t>
+  </si>
+  <si>
+    <t>SCP v2</t>
+  </si>
+  <si>
+    <t>✓</t>
+  </si>
+  <si>
+    <t>EventingCommand</t>
+  </si>
+  <si>
+    <t>Default: False</t>
+  </si>
+  <si>
+    <t>Fixed: True</t>
+  </si>
+  <si>
+    <t>streaming</t>
+  </si>
+  <si>
+    <t>retainsevents</t>
+  </si>
+  <si>
+    <t>Computed</t>
+  </si>
+  <si>
+    <t>generating</t>
+  </si>
+  <si>
+    <t>generates_timeorder</t>
+  </si>
+  <si>
+    <t>overrides_timeorder</t>
+  </si>
+  <si>
+    <t>requires_preop</t>
+  </si>
+  <si>
+    <t>streaming_preop</t>
+  </si>
+  <si>
+    <t>required_fields</t>
+  </si>
+  <si>
+    <t>clear_required_fields</t>
+  </si>
+  <si>
+    <t>distributed</t>
+  </si>
+  <si>
+    <t>maxinputs</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>Default: maxresultrows</t>
+  </si>
+  <si>
+    <t>Default: True</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Default: 'streaming'</t>
+  </si>
+  <si>
+    <t>Fixed: 'events'</t>
+  </si>
+  <si>
+    <t>Default: None</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -438,6 +560,18 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -452,7 +586,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -501,8 +635,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF660066"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="44">
+  <cellStyleXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -547,8 +690,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -575,8 +722,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="44">
+  <cellStyles count="48">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -598,6 +756,8 @@
     <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -619,10 +779,45 @@
     <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="29" builtinId="10"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color rgb="FF660066"/>
+        </top>
+        <bottom style="thin">
+          <color rgb="FF660066"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -651,6 +846,23 @@
     <tableColumn id="7" name="Overridable [SC]"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H13" totalsRowShown="0">
+  <autoFilter ref="A1:H13"/>
+  <tableColumns count="8">
+    <tableColumn id="1" name="Settiing" dataDxfId="1"/>
+    <tableColumn id="2" name="Type"/>
+    <tableColumn id="3" name="SCP v1" dataDxfId="0"/>
+    <tableColumn id="4" name="SCP v2"/>
+    <tableColumn id="5" name="EventingCommand"/>
+    <tableColumn id="6" name="GeneratingCommand"/>
+    <tableColumn id="7" name="ReportingCommand"/>
+    <tableColumn id="8" name="StreamingCommand"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -978,8 +1190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showRuler="0" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="B84" sqref="B84:B119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -2340,4 +2552,254 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.1640625" customWidth="1"/>
+    <col min="7" max="8" width="20.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="H2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="F4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" t="s">
+        <v>121</v>
+      </c>
+      <c r="H4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="G7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="G8" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9" t="s">
+        <v>141</v>
+      </c>
+      <c r="G9" t="s">
+        <v>141</v>
+      </c>
+      <c r="H9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="F11" t="s">
+        <v>121</v>
+      </c>
+      <c r="H11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B12" t="s">
+        <v>135</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="E12" t="s">
+        <v>136</v>
+      </c>
+      <c r="F12" t="s">
+        <v>136</v>
+      </c>
+      <c r="G12" t="s">
+        <v>136</v>
+      </c>
+      <c r="H12" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="18"/>
+      <c r="D13" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Hooked in all SCP v1 configuration settings
Decorator tests all pass.
</commit_message>
<xml_diff>
--- a/Commands.conf.spec.xlsx
+++ b/Commands.conf.spec.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="28260" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,84 @@
     <author>Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="G8" authorId="0">
+    <comment ref="C2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Selected fields mode is enabled when you specify required_fields and set this value to True
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Selected fields mode is enabled when required_fields are provided.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Selected fields mode is enabled when you specify required_fields and set this value to True
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Selected fields mode is enabled when you specify required_fields and set this value to True
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t xml:space="preserve">Selected fields mode is enabled when you specify required_fields and set this value to True
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Ignored unless type='streaming'. Only streaming commands can be distributed.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -45,15 +122,16 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0">
+    <comment ref="E14" authorId="0">
       <text>
         <r>
           <rPr>
+            <b/>
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
           </rPr>
-          <t>Ignored unless type='streaming'. Only streaming commands can be distributed.</t>
+          <t>TODO: Lobby for changing this name to 'eventing'</t>
         </r>
       </text>
     </comment>
@@ -81,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="146">
   <si>
     <t>type = &lt;string&gt;</t>
   </si>
@@ -506,14 +584,26 @@
     <t>Fixed: 'events'</t>
   </si>
   <si>
-    <t>Default: None</t>
+    <t>Fixed: 'reporting'</t>
+  </si>
+  <si>
+    <t>Fixed: 'streaming'</t>
+  </si>
+  <si>
+    <t>run_in_preview</t>
+  </si>
+  <si>
+    <t>list</t>
+  </si>
+  <si>
+    <t>Default: ['*']</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -572,6 +662,18 @@
       <color indexed="81"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -586,7 +688,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -635,17 +737,8 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF660066"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="48">
+  <cellStyleXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -694,8 +787,26 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -722,19 +833,22 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="48">
+  <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -758,6 +872,15 @@
     <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="63" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="65" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -781,16 +904,22 @@
     <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="62" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="64" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="29" builtinId="10"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -804,18 +933,9 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color rgb="FF660066"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FF660066"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -850,12 +970,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H13" totalsRowShown="0">
-  <autoFilter ref="A1:H13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:H14" totalsRowShown="0">
+  <autoFilter ref="A1:H14"/>
+  <sortState ref="A2:H14">
+    <sortCondition ref="A1:A14"/>
+  </sortState>
   <tableColumns count="8">
-    <tableColumn id="1" name="Settiing" dataDxfId="1"/>
+    <tableColumn id="1" name="Settiing" dataDxfId="0"/>
     <tableColumn id="2" name="Type"/>
-    <tableColumn id="3" name="SCP v1" dataDxfId="0"/>
+    <tableColumn id="3" name="SCP v1" dataDxfId="1"/>
     <tableColumn id="4" name="SCP v2"/>
     <tableColumn id="5" name="EventingCommand"/>
     <tableColumn id="6" name="GeneratingCommand"/>
@@ -1190,8 +1313,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84:B119"/>
+    <sheetView showRuler="0" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="B94" sqref="B94:B96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -2556,15 +2679,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H13"/>
+  <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="21.1640625" customWidth="1"/>
@@ -2598,205 +2721,238 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>123</v>
+      <c r="A2" s="14" t="s">
+        <v>132</v>
       </c>
       <c r="B2" t="s">
         <v>115</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="H2" t="s">
-        <v>122</v>
+      <c r="E2" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>137</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>124</v>
+      <c r="A3" s="19" t="s">
+        <v>133</v>
       </c>
       <c r="B3" t="s">
         <v>115</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="D3" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="E3" t="s">
-        <v>122</v>
+      <c r="F3" t="s">
+        <v>121</v>
+      </c>
+      <c r="H3" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>126</v>
+      <c r="A4" s="14" t="s">
+        <v>127</v>
       </c>
       <c r="B4" t="s">
         <v>115</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="D4" s="14" t="s">
-        <v>119</v>
-      </c>
       <c r="F4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G4" t="s">
         <v>121</v>
       </c>
-      <c r="H4" t="s">
-        <v>121</v>
-      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>127</v>
+      <c r="A5" s="14" t="s">
+        <v>126</v>
       </c>
       <c r="B5" t="s">
         <v>115</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="16" t="s">
         <v>119</v>
       </c>
+      <c r="D5" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" t="s">
+        <v>135</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E6" t="s">
+        <v>136</v>
+      </c>
+      <c r="F6" t="s">
+        <v>136</v>
+      </c>
+      <c r="G6" t="s">
+        <v>136</v>
+      </c>
+      <c r="H6" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
         <v>128</v>
-      </c>
-      <c r="B6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>129</v>
       </c>
       <c r="B7" t="s">
         <v>115</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>130</v>
+      <c r="A8" s="14" t="s">
+        <v>131</v>
       </c>
       <c r="B8" t="s">
-        <v>116</v>
-      </c>
-      <c r="C8" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="16" t="s">
         <v>119</v>
       </c>
+      <c r="E8" t="s">
+        <v>145</v>
+      </c>
       <c r="G8" t="s">
-        <v>125</v>
+        <v>145</v>
+      </c>
+      <c r="H8" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>131</v>
+      <c r="A9" s="14" t="s">
+        <v>129</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
-      </c>
-      <c r="C9" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="E9" t="s">
-        <v>141</v>
-      </c>
       <c r="G9" t="s">
-        <v>141</v>
-      </c>
-      <c r="H9" t="s">
-        <v>141</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>132</v>
+      <c r="A10" s="14" t="s">
+        <v>124</v>
       </c>
       <c r="B10" t="s">
         <v>115</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="16" t="s">
         <v>119</v>
       </c>
+      <c r="E10" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="15" t="s">
-        <v>133</v>
+      <c r="A11" s="19" t="s">
+        <v>143</v>
       </c>
       <c r="B11" t="s">
         <v>115</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="C11" s="16"/>
+      <c r="D11" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="F11" t="s">
-        <v>121</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="G11" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>134</v>
+      <c r="A12" s="14" t="s">
+        <v>123</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
-      </c>
-      <c r="D12" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C12" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="E12" t="s">
-        <v>136</v>
-      </c>
-      <c r="F12" t="s">
-        <v>136</v>
-      </c>
-      <c r="G12" t="s">
-        <v>136</v>
-      </c>
       <c r="H12" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
-        <v>138</v>
-      </c>
-      <c r="B13" s="10" t="s">
+      <c r="A13" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" t="s">
         <v>116</v>
       </c>
-      <c r="C13" s="18"/>
+      <c r="C13" s="16" t="s">
+        <v>119</v>
+      </c>
       <c r="D13" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="G13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C14" s="18"/>
+      <c r="D14" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
+      <c r="G14" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>142</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>

</xml_diff>